<commit_message>
Projet fini avec document
</commit_message>
<xml_diff>
--- a/Journal de veille.xlsx
+++ b/Journal de veille.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wille\Documents\Projet Final\Approfondissement2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wille\Documents\CodeLaravel\meteoapi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35C4593D-1611-4FB1-8E0D-D8B9022045A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5B102B6-CB97-4922-AC5C-C278B55B4FE4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="46">
   <si>
     <t>Source</t>
   </si>
@@ -97,7 +97,73 @@
     <t>c'est le site de documentation que l'api fournit https://docs.google.com/document/d/1_Zte7-SdOjnzBttb1-Y9e0Wgl0_3tah9dSwXUyEA3-c/edit</t>
   </si>
   <si>
-    <t>c'est le site de documentation que l'api fournit https://docs.google.com/document/d/1GsvGH7TEog_z63ZawX0lHohISBv4qb0aIh8WoHHINF0/edit </t>
+    <t>C'est un site d'apprentissage qui a beaucoup de documentation https://www.w3schools.com/python/python_variables_global.asp</t>
+  </si>
+  <si>
+    <t>C'est un site d'apprentissage qui a beaucoup de documentation sur pyqt https://www.learnpyqt.com/tutorials/creating-multiple-windows/</t>
+  </si>
+  <si>
+    <t>learnpyqt.com</t>
+  </si>
+  <si>
+    <t>C'est un site de documentation varié https://www.geeksforgeeks.org/g-fact-41-multiple-return-values-in-python/</t>
+  </si>
+  <si>
+    <t>Geekforgeeks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forum </t>
+  </si>
+  <si>
+    <t>Stackoverflow</t>
+  </si>
+  <si>
+    <t>C'est un forum auquel plusieurs solutions sont proposées https://stackoverflow.com/questions/181530/styling-multi-line-conditions-in-if-statements</t>
+  </si>
+  <si>
+    <t>c'est un forum auquel plusieurs solution sont proposées https://stackoverflow.com/questions/51821498/pyqt5-changing-images</t>
+  </si>
+  <si>
+    <t>J'ai souvent eu à regarder le type d'un élément car il fallait être précis https://realpython.com/python-type-checking/</t>
+  </si>
+  <si>
+    <t>RealPython</t>
+  </si>
+  <si>
+    <t>Documentation officiel de python https://docs.python.org/fr/3/tutorial/classes.html</t>
+  </si>
+  <si>
+    <t>Documentation Python</t>
+  </si>
+  <si>
+    <t>c'est le site de documentation que l'api fournit https://docs.google.com/document/d/1GsvGH7TEog_z63ZawX0lHohISBv4qb0aIh8WoHHINF0/edit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Montre comment le lien url est composé et les éléments à changer afin de pouvoir utiliser les prévisions métérologiques des journées précédentes (Maximum de 7). Puis ensuite décrit les éléments qui seront retourner avec un exemple.  </t>
+  </si>
+  <si>
+    <t>C'est un cours qu'un docteur et a obtenu un diplome universitaire en web qui montre comment pyqt fonctionne et les bases</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Montre comment les variables globales fonctionne avec un exemple. </t>
+  </si>
+  <si>
+    <t>Montre comment avoir un logiciel avec plusieurs interface dans pyqt et pour interchanger des valeurs dedans.</t>
+  </si>
+  <si>
+    <t>Montre comment retourner plusieurs valeurs d'une fonction en python.</t>
+  </si>
+  <si>
+    <t>Montre comment changer l'image d'une icone.</t>
+  </si>
+  <si>
+    <t>Montre comment associer plusieurs conditions a un if statement en python.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Montre comment afficher le type d'un champs ce qui m'a aider à avoir moins d'erreur. </t>
+  </si>
+  <si>
+    <t>Montre comment une classe fonctionne et m'a permis de voir comment les importés.</t>
   </si>
 </sst>
 </file>
@@ -398,9 +464,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -423,6 +486,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -708,8 +774,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G232"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -734,19 +800,19 @@
     </row>
     <row r="2" spans="1:7" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="14"/>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="D2" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="E2" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="26" t="s">
+      <c r="F2" s="25" t="s">
         <v>4</v>
       </c>
       <c r="G2" s="5"/>
@@ -759,10 +825,10 @@
       <c r="C3" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="30" t="s">
+      <c r="D3" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="28">
+      <c r="E3" s="27">
         <v>44221</v>
       </c>
       <c r="F3" s="16" t="s">
@@ -778,10 +844,10 @@
       <c r="C4" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="30" t="s">
+      <c r="D4" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="29">
+      <c r="E4" s="28">
         <v>44222</v>
       </c>
       <c r="F4" s="18" t="s">
@@ -797,10 +863,10 @@
       <c r="C5" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="30" t="s">
+      <c r="D5" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="29">
+      <c r="E5" s="28">
         <v>44223</v>
       </c>
       <c r="F5" s="18" t="s">
@@ -816,10 +882,10 @@
       <c r="C6" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="30" t="s">
+      <c r="D6" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="29">
+      <c r="E6" s="28">
         <v>44224</v>
       </c>
       <c r="F6" s="19" t="s">
@@ -835,10 +901,10 @@
       <c r="C7" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="30" t="s">
+      <c r="D7" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="29">
+      <c r="E7" s="28">
         <v>44225</v>
       </c>
       <c r="F7" s="18" t="s">
@@ -854,10 +920,10 @@
       <c r="C8" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="30" t="s">
+      <c r="D8" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="29">
+      <c r="E8" s="28">
         <v>44228</v>
       </c>
       <c r="F8" s="18" t="s">
@@ -865,7 +931,7 @@
       </c>
       <c r="G8" s="5"/>
     </row>
-    <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="17" t="s">
         <v>8</v>
@@ -873,89 +939,167 @@
       <c r="C9" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" s="19"/>
-      <c r="F9" s="18"/>
+      <c r="D9" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" s="28">
+        <v>44229</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>37</v>
+      </c>
       <c r="G9" s="5"/>
     </row>
-    <row r="10" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="27" t="s">
+      <c r="C10" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="27" t="s">
+      <c r="D10" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="19"/>
-      <c r="F10" s="18"/>
+      <c r="E10" s="28">
+        <v>44230</v>
+      </c>
+      <c r="F10" s="18" t="s">
+        <v>38</v>
+      </c>
       <c r="G10" s="5"/>
     </row>
     <row r="11" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="18"/>
+      <c r="B11" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="28">
+        <v>44231</v>
+      </c>
+      <c r="F11" s="18" t="s">
+        <v>39</v>
+      </c>
       <c r="G11" s="5"/>
     </row>
     <row r="12" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="18"/>
+      <c r="B12" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="28">
+        <v>44232</v>
+      </c>
+      <c r="F12" s="18" t="s">
+        <v>40</v>
+      </c>
       <c r="G12" s="5"/>
     </row>
     <row r="13" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="18"/>
+      <c r="B13" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="28">
+        <v>44235</v>
+      </c>
+      <c r="F13" s="18" t="s">
+        <v>41</v>
+      </c>
       <c r="G13" s="5"/>
     </row>
     <row r="14" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="18"/>
+      <c r="B14" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" s="28">
+        <v>44236</v>
+      </c>
+      <c r="F14" s="18" t="s">
+        <v>42</v>
+      </c>
       <c r="G14" s="5"/>
     </row>
     <row r="15" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="18"/>
+      <c r="B15" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" s="28">
+        <v>44237</v>
+      </c>
+      <c r="F15" s="18" t="s">
+        <v>43</v>
+      </c>
       <c r="G15" s="5"/>
     </row>
     <row r="16" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
-      <c r="B16" s="17"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="18"/>
+      <c r="B16" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" s="28">
+        <v>44238</v>
+      </c>
+      <c r="F16" s="18" t="s">
+        <v>44</v>
+      </c>
       <c r="G16" s="5"/>
     </row>
     <row r="17" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="11"/>
-      <c r="B17" s="20"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="22"/>
-      <c r="F17" s="21"/>
+      <c r="B17" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="E17" s="28">
+        <v>44239</v>
+      </c>
+      <c r="F17" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="G17" s="5"/>
     </row>
     <row r="18" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2258,8 +2402,15 @@
     <hyperlink ref="D7" r:id="rId7" display="https://docs.google.com/document/d/1KGb8bTVYRsNgljnNH67AMhckY8AQT2FVwZ9urj8SWBs/edit" xr:uid="{8842C07B-B579-4288-93B2-51227B2F8634}"/>
     <hyperlink ref="D8" r:id="rId8" display="https://docs.google.com/document/d/1_Zte7-SdOjnzBttb1-Y9e0Wgl0_3tah9dSwXUyEA3-c/edit" xr:uid="{5EFDF831-4DA9-4A73-85F0-BE0A7FBFF4BB}"/>
     <hyperlink ref="D9" r:id="rId9" display="https://docs.google.com/document/d/1GsvGH7TEog_z63ZawX0lHohISBv4qb0aIh8WoHHINF0/edit " xr:uid="{B29FCF45-5A9F-4F25-A56C-47F7D80E61AD}"/>
+    <hyperlink ref="D11" r:id="rId10" display="https://www.w3schools.com/python/python_variables_global.asp" xr:uid="{486342A9-561B-4522-B87A-82D5D859E2CC}"/>
+    <hyperlink ref="D12" r:id="rId11" xr:uid="{B129E2AF-BDF4-4D12-9AC3-722BD61ED796}"/>
+    <hyperlink ref="D13" r:id="rId12" xr:uid="{2BDC9D9C-3C95-4A8E-9BF7-D98BE20DFBBC}"/>
+    <hyperlink ref="D14" r:id="rId13" display="c'est un site de forum auquel plusieurs solution sont proposées https://stackoverflow.com/questions/51821498/pyqt5-changing-images" xr:uid="{DAFF251E-0866-454C-A70A-C47AB4143AD9}"/>
+    <hyperlink ref="D15" r:id="rId14" xr:uid="{373192C7-2C46-4EE7-B29C-8E93F175D559}"/>
+    <hyperlink ref="D16" r:id="rId15" xr:uid="{1D187395-3AB5-4542-A0D4-3DDBCBBEE419}"/>
+    <hyperlink ref="D17" r:id="rId16" xr:uid="{3AE8322C-92B6-47E3-B207-4247C5F14615}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId10"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId17"/>
 </worksheet>
 </file>
</xml_diff>